<commit_message>
Update Burndown Chart in Team Report
</commit_message>
<xml_diff>
--- a/Team02Report.xlsx
+++ b/Team02Report.xlsx
@@ -5,26 +5,27 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\2021S-CS-555-A-Agile_methods_For_sw_dev\Project\Sprint 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\prash\Coding\Stevens\CS555\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7951EDE9-D288-418E-B188-D9D49D267B66}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70931015-C237-42BA-860E-C4FB137EFE11}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5100" yWindow="5145" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
     <sheet name="Backlog" sheetId="6" r:id="rId2"/>
+    <sheet name="Burndown" sheetId="2" r:id="rId3"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId3"/>
+    <externalReference r:id="rId4"/>
   </externalReferences>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="80">
   <si>
     <t>Coding</t>
   </si>
@@ -173,6 +174,36 @@
     <t xml:space="preserve">Initial </t>
   </si>
   <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Remaining Stories</t>
+  </si>
+  <si>
+    <t>Story Velocity</t>
+  </si>
+  <si>
+    <t>LOC</t>
+  </si>
+  <si>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Code Velocity</t>
+  </si>
+  <si>
+    <t>Start</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    03-01-2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sprint 1 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">    03-17-2021</t>
+  </si>
+  <si>
     <t>CS555-AgileProject-Group2</t>
   </si>
   <si>
@@ -228,6 +259,9 @@
   </si>
   <si>
     <t>Backlog Details</t>
+  </si>
+  <si>
+    <t>Burndown Chart for Competed Sprints and Remaining Stories</t>
   </si>
   <si>
     <t>Project Team Details</t>
@@ -383,7 +417,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -406,9 +440,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -429,6 +471,1792 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>BURN DOWN chart</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>[1]Sheet2!$D$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Remaining Stories</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="22225" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="50000"/>
+                        <a:lumOff val="50000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>[1]Sheet2!$B$4:$C$5</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="2"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>    03-01-2021</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>    03-17-2021</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Start</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Sprint 1 </c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>[1]Sheet2!$D$4:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-67FE-497C-B527-7002BAAE672A}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="145513856"/>
+        <c:axId val="145552896"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$E$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Story Velocity</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="square"/>
+                  <c:size val="6"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent2"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="50000"/>
+                              <a:lumOff val="50000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="t"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst>
+                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$B$4:$C$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="2"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>    03-01-2021</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>    03-17-2021</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Start</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Sprint 1 </c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$E$4:$E$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="1">
+                        <c:v>8</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-67FE-497C-B527-7002BAAE672A}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="2"/>
+                <c:order val="2"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$F$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>LOC</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="triangle"/>
+                  <c:size val="6"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent3"/>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent3"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="50000"/>
+                              <a:lumOff val="50000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="t"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$B$4:$C$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="2"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>    03-01-2021</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>    03-17-2021</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Start</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Sprint 1 </c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$F$4:$F$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>0</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>240</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000002-67FE-497C-B527-7002BAAE672A}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$G$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Min</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="x"/>
+                  <c:size val="6"/>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="50000"/>
+                              <a:lumOff val="50000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="t"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$B$4:$C$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="2"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>    03-01-2021</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>    03-17-2021</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Start</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Sprint 1 </c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$G$4:$G$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="1">
+                        <c:v>480</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-67FE-497C-B527-7002BAAE672A}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="4"/>
+                <c:order val="4"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$H$3</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>Code Velocity</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="22225" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent5"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="star"/>
+                  <c:size val="6"/>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent5"/>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:dLbls>
+                  <c:spPr>
+                    <a:noFill/>
+                    <a:ln>
+                      <a:noFill/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                  <c:txPr>
+                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                      <a:spAutoFit/>
+                    </a:bodyPr>
+                    <a:lstStyle/>
+                    <a:p>
+                      <a:pPr>
+                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                          <a:solidFill>
+                            <a:schemeClr val="tx1">
+                              <a:lumMod val="50000"/>
+                              <a:lumOff val="50000"/>
+                            </a:schemeClr>
+                          </a:solidFill>
+                          <a:latin typeface="+mn-lt"/>
+                          <a:ea typeface="+mn-ea"/>
+                          <a:cs typeface="+mn-cs"/>
+                        </a:defRPr>
+                      </a:pPr>
+                      <a:endParaRPr lang="en-US"/>
+                    </a:p>
+                  </c:txPr>
+                  <c:dLblPos val="t"/>
+                  <c:showLegendKey val="0"/>
+                  <c:showVal val="1"/>
+                  <c:showCatName val="0"/>
+                  <c:showSerName val="0"/>
+                  <c:showPercent val="0"/>
+                  <c:showBubbleSize val="0"/>
+                  <c:showLeaderLines val="0"/>
+                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                      <c15:showLeaderLines val="1"/>
+                      <c15:leaderLines>
+                        <c:spPr>
+                          <a:ln w="9525">
+                            <a:solidFill>
+                              <a:schemeClr val="tx1">
+                                <a:lumMod val="35000"/>
+                                <a:lumOff val="65000"/>
+                              </a:schemeClr>
+                            </a:solidFill>
+                          </a:ln>
+                          <a:effectLst/>
+                        </c:spPr>
+                      </c15:leaderLines>
+                    </c:ext>
+                  </c:extLst>
+                </c:dLbls>
+                <c:cat>
+                  <c:multiLvlStrRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$B$4:$C$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:multiLvlStrCache>
+                      <c:ptCount val="2"/>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>    03-01-2021</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>    03-17-2021</c:v>
+                        </c:pt>
+                      </c:lvl>
+                      <c:lvl>
+                        <c:pt idx="0">
+                          <c:v>Start</c:v>
+                        </c:pt>
+                        <c:pt idx="1">
+                          <c:v>Sprint 1 </c:v>
+                        </c:pt>
+                      </c:lvl>
+                    </c:multiLvlStrCache>
+                  </c:multiLvlStrRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>[1]Sheet2!$H$4:$H$5</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="2"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000004-67FE-497C-B527-7002BAAE672A}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="145513856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>dates</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="145552896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="145552896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN" baseline="0"/>
+                  <a:t>rEMAINING stories</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-IN"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.6666666666666673E-2"/>
+              <c:y val="0.30253827646544196"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="dk1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="145513856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="lt1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="239">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="800" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="800" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>396875</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>92075</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>447675</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>73025</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DD35CEC-24C0-4E18-8138-631ACCAB9487}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -823,24 +2651,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:F11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="4" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="29.33203125" customWidth="1"/>
-    <col min="6" max="6" width="27.6640625" customWidth="1"/>
+    <col min="3" max="4" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="29.28515625" customWidth="1"/>
+    <col min="6" max="6" width="27.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="18" x14ac:dyDescent="0.35">
-      <c r="E3" s="15" t="s">
-        <v>68</v>
+    <row r="3" spans="2:6" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="E3" s="19" t="s">
+        <v>79</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>48</v>
       </c>
@@ -857,7 +2685,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>18</v>
       </c>
@@ -874,7 +2702,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
@@ -891,7 +2719,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>7</v>
       </c>
@@ -908,7 +2736,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>15</v>
       </c>
@@ -925,7 +2753,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B10" s="8"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
@@ -933,10 +2761,10 @@
         <v>27</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
-    <row r="11" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -959,34 +2787,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="6" max="6" width="30.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="F2" s="16" t="s">
-        <v>67</v>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="F2" s="20" t="s">
+        <v>77</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="14"/>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="16"/>
       <c r="C4" s="1" t="s">
         <v>26</v>
       </c>
@@ -1003,9 +2831,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="14"/>
-      <c r="C5" s="14">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+      <c r="C5" s="16">
         <v>1</v>
       </c>
       <c r="D5" t="s">
@@ -1018,12 +2846,12 @@
         <v>20</v>
       </c>
       <c r="G5" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="14"/>
-      <c r="C6" s="14">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="16"/>
+      <c r="C6" s="16">
         <v>1</v>
       </c>
       <c r="D6" t="s">
@@ -1036,12 +2864,12 @@
         <v>17</v>
       </c>
       <c r="G6" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
-      <c r="C7" s="14">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+      <c r="C7" s="16">
         <v>1</v>
       </c>
       <c r="D7" t="s">
@@ -1054,12 +2882,12 @@
         <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="14"/>
-      <c r="C8" s="14">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="16"/>
+      <c r="C8" s="16">
         <v>1</v>
       </c>
       <c r="D8" t="s">
@@ -1072,12 +2900,12 @@
         <v>11</v>
       </c>
       <c r="G8" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="14"/>
-      <c r="C9" s="14">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+      <c r="C9" s="16">
         <v>1</v>
       </c>
       <c r="D9" t="s">
@@ -1090,11 +2918,11 @@
         <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="14">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="16">
         <v>1</v>
       </c>
       <c r="D10" t="s">
@@ -1107,11 +2935,11 @@
         <v>6</v>
       </c>
       <c r="G10" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C11" s="14">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="16">
         <v>1</v>
       </c>
       <c r="D11" t="s">
@@ -1124,11 +2952,11 @@
         <v>4</v>
       </c>
       <c r="G11" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C12" s="14">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="16">
         <v>1</v>
       </c>
       <c r="D12" t="s">
@@ -1141,140 +2969,140 @@
         <v>1</v>
       </c>
       <c r="G12" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C13" s="14">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C13" s="16">
         <v>2</v>
       </c>
       <c r="D13" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="E13" t="s">
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="G13" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C14" s="14">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C14" s="16">
         <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="G14" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C15" s="14">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C15" s="16">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="E15" t="s">
         <v>18</v>
       </c>
       <c r="F15" t="s">
-        <v>61</v>
+        <v>71</v>
       </c>
       <c r="G15" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="14">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="16">
         <v>2</v>
       </c>
       <c r="D16" t="s">
-        <v>54</v>
+        <v>64</v>
       </c>
       <c r="E16" t="s">
         <v>18</v>
       </c>
       <c r="F16" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="G16" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C17" s="14">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="16">
         <v>2</v>
       </c>
       <c r="D17" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="E17" t="s">
         <v>15</v>
       </c>
       <c r="F17" t="s">
-        <v>63</v>
+        <v>73</v>
       </c>
       <c r="G17" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C18" s="14">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="16">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="E18" t="s">
         <v>15</v>
       </c>
       <c r="F18" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="G18" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C19" s="14">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="16">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>67</v>
       </c>
       <c r="E19" t="s">
         <v>7</v>
       </c>
       <c r="F19" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="G19" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C20" s="14">
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20" s="16">
         <v>2</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="E20" t="s">
         <v>7</v>
       </c>
       <c r="F20" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="G20" t="s">
         <v>0</v>
@@ -1284,4 +3112,95 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="D2:K7"/>
+  <sheetViews>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="4:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="F2" s="18" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D5" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="G5" s="15" t="s">
+        <v>51</v>
+      </c>
+      <c r="H5" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D6" t="s">
+        <v>55</v>
+      </c>
+      <c r="E6" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="16">
+        <v>32</v>
+      </c>
+      <c r="H6" s="16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>57</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="16">
+        <v>24</v>
+      </c>
+      <c r="G7" s="16">
+        <v>8</v>
+      </c>
+      <c r="H7" s="16">
+        <v>190</v>
+      </c>
+      <c r="I7" s="16">
+        <v>300</v>
+      </c>
+      <c r="J7" s="16">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Team Report Sprint 2
</commit_message>
<xml_diff>
--- a/Team02Report.xlsx
+++ b/Team02Report.xlsx
@@ -1,95 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shubh\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFDEC4B5-DE48-4523-8214-126FE3DB6B02}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="4"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
     <sheet name="Backlog" sheetId="6" r:id="rId2"/>
     <sheet name="Burndown" sheetId="2" r:id="rId3"/>
-    <sheet name="Sprint1" sheetId="4" r:id="rId4"/>
-    <sheet name="Sprint2" sheetId="5" r:id="rId5"/>
+    <sheet name="Sprint 2" sheetId="4" r:id="rId4"/>
+    <sheet name="Sprint 3" sheetId="5" r:id="rId5"/>
   </sheets>
   <externalReferences>
     <externalReference r:id="rId6"/>
   </externalReferences>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Burndown!$D$6:$E$8</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Burndown!$F$5</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Burndown!$J$6:$J$8</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Burndown!$F$6:$F$8</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Burndown!$G$5</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Burndown!$G$6:$G$8</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Burndown!$H$5</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Burndown!$H$6:$H$8</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Burndown!$I$5</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Burndown!$I$6:$I$8</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Burndown!$J$5</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="129">
   <si>
     <t>Coding</t>
   </si>
   <si>
-    <t>Birth before marriage of parents</t>
-  </si>
-  <si>
     <t>MS</t>
   </si>
   <si>
-    <t>US08</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Less then 150 years old </t>
-  </si>
-  <si>
-    <t>US07</t>
-  </si>
-  <si>
-    <t>Divorce before death</t>
-  </si>
-  <si>
     <t>SS</t>
   </si>
   <si>
-    <t>US06</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marriage before death </t>
-  </si>
-  <si>
-    <t>US05</t>
-  </si>
-  <si>
-    <t>Marriage before divorce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SM </t>
-  </si>
-  <si>
-    <t>US04</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Birth before death </t>
-  </si>
-  <si>
     <t>SM</t>
   </si>
   <si>
-    <t xml:space="preserve">US03 </t>
-  </si>
-  <si>
-    <t>Birth before marriage</t>
-  </si>
-  <si>
     <t>PM</t>
   </si>
   <si>
-    <t>US02</t>
-  </si>
-  <si>
-    <t>Dates before currennt date</t>
-  </si>
-  <si>
-    <t>US01</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -216,27 +183,6 @@
     <t>Completed</t>
   </si>
   <si>
-    <t>Dates before current date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Birth before marriage </t>
-  </si>
-  <si>
-    <t>US03</t>
-  </si>
-  <si>
-    <t>Birth before death</t>
-  </si>
-  <si>
-    <t xml:space="preserve">US07 </t>
-  </si>
-  <si>
-    <t>Less then 150 years old</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Birth before marriage of parents </t>
-  </si>
-  <si>
     <t>CS555-AgileProject-Group2</t>
   </si>
   <si>
@@ -252,9 +198,6 @@
     <t xml:space="preserve">Story Name </t>
   </si>
   <si>
-    <t xml:space="preserve">Overview of Sprint 2 </t>
-  </si>
-  <si>
     <t>US09</t>
   </si>
   <si>
@@ -303,12 +246,6 @@
     <t>Male last names</t>
   </si>
   <si>
-    <t>03/17/2021</t>
-  </si>
-  <si>
-    <t>Completed Sprint 1 User Stories</t>
-  </si>
-  <si>
     <t>Backlog Details</t>
   </si>
   <si>
@@ -318,63 +255,6 @@
     <t>Project Team Details</t>
   </si>
   <si>
-    <t>T08.01</t>
-  </si>
-  <si>
-    <t>Store Marriage date</t>
-  </si>
-  <si>
-    <t>T08.02</t>
-  </si>
-  <si>
-    <t>Store Divorce date</t>
-  </si>
-  <si>
-    <t>T08.03</t>
-  </si>
-  <si>
-    <t>Child's birth date should fall between Marriage date and 9 months after divorce date</t>
-  </si>
-  <si>
-    <t>T07.01</t>
-  </si>
-  <si>
-    <t>Store Death date of dead people less than 150 years</t>
-  </si>
-  <si>
-    <t>T07.02</t>
-  </si>
-  <si>
-    <t>Store Birth date of people</t>
-  </si>
-  <si>
-    <t>T07.03</t>
-  </si>
-  <si>
-    <t>Current date should be less than 150 years after birth date</t>
-  </si>
-  <si>
-    <t>T06.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Store Death date of Husband </t>
-  </si>
-  <si>
-    <t>T06.02</t>
-  </si>
-  <si>
-    <t>Store Death date of Wife</t>
-  </si>
-  <si>
-    <t>T06.03</t>
-  </si>
-  <si>
-    <t>Store Divorce date before death dates of Spouses</t>
-  </si>
-  <si>
-    <t>T05.01</t>
-  </si>
-  <si>
     <t>Keep Doing:</t>
   </si>
   <si>
@@ -390,89 +270,170 @@
     <t>Leaving leftover pizza on the counter</t>
   </si>
   <si>
-    <t>T05.02</t>
-  </si>
-  <si>
-    <t>T04.01</t>
-  </si>
-  <si>
     <t>Bring pizza to our meetings</t>
   </si>
   <si>
-    <t>Store Divorce date of either spouses</t>
-  </si>
-  <si>
-    <t>T04.02</t>
-  </si>
-  <si>
-    <t>T04.03</t>
-  </si>
-  <si>
-    <t>Store Divorce date after Marriage date</t>
-  </si>
-  <si>
-    <t>Store Marriage date of the spouses before Divorce date</t>
-  </si>
-  <si>
-    <t>T03.01</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Store Birth date </t>
-  </si>
-  <si>
-    <t>T03.02</t>
-  </si>
-  <si>
-    <t>Store Death date</t>
-  </si>
-  <si>
-    <t>T03.03</t>
-  </si>
-  <si>
-    <t>Compare Birth and Death dates</t>
-  </si>
-  <si>
-    <t>T02.01</t>
-  </si>
-  <si>
-    <t>Store Birth date</t>
-  </si>
-  <si>
-    <t>T02.02</t>
-  </si>
-  <si>
-    <t>Store Marriage date after Birth date</t>
-  </si>
-  <si>
-    <t>T01.01</t>
-  </si>
-  <si>
-    <t>Store Current date</t>
-  </si>
-  <si>
-    <t>Store Birth, Marriage and Divorce dates</t>
-  </si>
-  <si>
-    <t>Compare Birth, Marriage and Divorce dates with the current date</t>
-  </si>
-  <si>
-    <t>Find Marriage record for an individual</t>
-  </si>
-  <si>
-    <t>Find Marriage date</t>
-  </si>
-  <si>
-    <t>T05.03</t>
-  </si>
-  <si>
-    <t>Compare Marriage date to Birth date</t>
+    <t>Sprint 2</t>
+  </si>
+  <si>
+    <t>03-29-2021</t>
+  </si>
+  <si>
+    <t>Completed Sprint 2 User Stories</t>
+  </si>
+  <si>
+    <t>03/29/2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">US15 </t>
+  </si>
+  <si>
+    <t>US17</t>
+  </si>
+  <si>
+    <t>US18</t>
+  </si>
+  <si>
+    <t>US19</t>
+  </si>
+  <si>
+    <t>US20</t>
+  </si>
+  <si>
+    <t>US21</t>
+  </si>
+  <si>
+    <t>US22</t>
+  </si>
+  <si>
+    <t>US23</t>
+  </si>
+  <si>
+    <t>US24</t>
+  </si>
+  <si>
+    <t>No marriages to descendants</t>
+  </si>
+  <si>
+    <t>Siblings should not marry</t>
+  </si>
+  <si>
+    <t>First cousins should not marry</t>
+  </si>
+  <si>
+    <t>Aunts and uncles</t>
+  </si>
+  <si>
+    <t>Correct gender for role</t>
+  </si>
+  <si>
+    <t>Unique IDs</t>
+  </si>
+  <si>
+    <t>Unique name and birthdate</t>
+  </si>
+  <si>
+    <t>Unique families by spouses</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overview of Sprint 3 </t>
+  </si>
+  <si>
+    <t>Implementation and Integration of User Story 9 where birth date should be before the death date of either parents</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Implementing User Story 10 where the marriage date should not be before the age of 14</t>
+  </si>
+  <si>
+    <t>T09</t>
+  </si>
+  <si>
+    <t>T10</t>
+  </si>
+  <si>
+    <t>T11</t>
+  </si>
+  <si>
+    <t>T12.01</t>
+  </si>
+  <si>
+    <t>Store children birth date</t>
+  </si>
+  <si>
+    <t>T12.02</t>
+  </si>
+  <si>
+    <t>T12.03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Siblings spacing </t>
+  </si>
+  <si>
+    <t>T13.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store birth date of siblings more than 8 months apart </t>
+  </si>
+  <si>
+    <t>T13.02</t>
+  </si>
+  <si>
+    <t>Store birth date of siblings less than 2 days apart (for twins)</t>
+  </si>
+  <si>
+    <t>T13.03</t>
+  </si>
+  <si>
+    <t>T14.01</t>
+  </si>
+  <si>
+    <t>Store the number of siblings which should not be more than 5</t>
+  </si>
+  <si>
+    <t>T14.02</t>
+  </si>
+  <si>
+    <t>T15.01</t>
+  </si>
+  <si>
+    <t>Store the number of siblings not more than 15</t>
+  </si>
+  <si>
+    <t>T16.01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Store the last name of the family </t>
+  </si>
+  <si>
+    <t>T16.02</t>
+  </si>
+  <si>
+    <t>Compare and implementing the last name of the male members</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compare and implementing the birth dates of siblings </t>
+  </si>
+  <si>
+    <t>Compare and implementing the birth dates of siblings</t>
+  </si>
+  <si>
+    <t>Compare and implementing birth date of mother less than 60 years of that of children birth date</t>
+  </si>
+  <si>
+    <t>Compare and implementing birth date of father less than 80 years of that of children birth date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Compare and implement the current marriage date which  should not appear before any of the previous marriage date of either spouses </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -499,15 +460,6 @@
       <b/>
       <u/>
       <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -663,7 +615,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -683,8 +637,18 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
   <c:chart>
     <c:title>
       <c:tx>
@@ -706,14 +670,13 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>BURN DOWN chart</a:t>
+              <a:rPr lang="en-US"/>
+              <a:t>Burn Down Chart</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -721,17 +684,39 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
     </c:title>
+    <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
-        <c:grouping val="stacked"/>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>[1]Sheet2!$D$3</c:f>
+              <c:f>Burndown!$F$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -765,68 +750,20 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
-          <c:dLbls>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="50000"/>
-                        <a:lumOff val="50000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:dLblPos val="t"/>
-            <c:showVal val="1"/>
-            <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>[1]Sheet2!$B$4:$C$5</c:f>
+              <c:f>Burndown!$D$6:$E$8</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:lvl>
                   <c:pt idx="0">
-                    <c:v>Sprint 1 </c:v>
+                    <c:v>    03-01-2021</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>    03-17-2021</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>03-29-2021</c:v>
                   </c:pt>
                 </c:lvl>
                 <c:lvl>
@@ -834,7 +771,10 @@
                     <c:v>Start</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>    03-01-2021</c:v>
+                    <c:v>Sprint 1 </c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Sprint 2</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -842,32 +782,42 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>[1]Sheet2!$D$4:$D$5</c:f>
+              <c:f>Burndown!$F$6:$F$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>24</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:smooth val="0"/>
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-67FE-497C-B527-7002BAAE672A}"/>
+              <c16:uniqueId val="{00000000-4D37-42F5-A377-6318DE2B5F0D}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:showVal val="1"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:marker val="1"/>
-        <c:axId val="145513856"/>
-        <c:axId val="145552896"/>
-        <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+        <c:smooth val="0"/>
+        <c:axId val="516104256"/>
+        <c:axId val="516110488"/>
+        <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredLineSeries>
               <c15:ser>
@@ -878,7 +828,7 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>[1]Sheet2!$E$3</c15:sqref>
+                          <c15:sqref>Burndown!$G$5</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -900,95 +850,28 @@
                   <a:effectLst/>
                 </c:spPr>
                 <c:marker>
-                  <c:symbol val="square"/>
-                  <c:size val="6"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent2"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent2"/>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
+                  <c:symbol val="none"/>
                 </c:marker>
-                <c:dLbls>
-                  <c:spPr>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                  <c:txPr>
-                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                      <a:spAutoFit/>
-                    </a:bodyPr>
-                    <a:lstStyle/>
-                    <a:p>
-                      <a:pPr>
-                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="50000"/>
-                              <a:lumOff val="50000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                          <a:latin typeface="+mn-lt"/>
-                          <a:ea typeface="+mn-ea"/>
-                          <a:cs typeface="+mn-cs"/>
-                        </a:defRPr>
-                      </a:pPr>
-                      <a:endParaRPr lang="en-US"/>
-                    </a:p>
-                  </c:txPr>
-                  <c:dLblPos val="t"/>
-                  <c:showLegendKey val="0"/>
-                  <c:showVal val="1"/>
-                  <c:showCatName val="0"/>
-                  <c:showSerName val="0"/>
-                  <c:showPercent val="0"/>
-                  <c:showBubbleSize val="0"/>
-                  <c:showLeaderLines val="0"/>
-                  <c:extLst>
-                    <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                      <c15:showLeaderLines val="1"/>
-                      <c15:leaderLines>
-                        <c:spPr>
-                          <a:ln w="9525">
-                            <a:solidFill>
-                              <a:schemeClr val="tx1">
-                                <a:lumMod val="35000"/>
-                                <a:lumOff val="65000"/>
-                              </a:schemeClr>
-                            </a:solidFill>
-                          </a:ln>
-                          <a:effectLst/>
-                        </c:spPr>
-                      </c15:leaderLines>
-                    </c:ext>
-                  </c:extLst>
-                </c:dLbls>
                 <c:cat>
                   <c:multiLvlStrRef>
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>[1]Sheet2!$B$4:$C$5</c15:sqref>
+                          <c15:sqref>Burndown!$D$6:$E$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="2"/>
+                      <c:ptCount val="3"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>    03-01-2021</c:v>
                         </c:pt>
                         <c:pt idx="1">
                           <c:v>    03-17-2021</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>03-29-2021</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -997,6 +880,9 @@
                         </c:pt>
                         <c:pt idx="1">
                           <c:v>Sprint 1 </c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Sprint 2</c:v>
                         </c:pt>
                       </c:lvl>
                     </c:multiLvlStrCache>
@@ -1007,14 +893,17 @@
                     <c:extLst>
                       <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>[1]Sheet2!$E$4:$E$5</c15:sqref>
+                          <c15:sqref>Burndown!$G$6:$G$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
+                      <c:ptCount val="3"/>
                       <c:pt idx="1">
+                        <c:v>8</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
                         <c:v>8</c:v>
                       </c:pt>
                     </c:numCache>
@@ -1023,7 +912,7 @@
                 <c:smooth val="0"/>
                 <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000001-67FE-497C-B527-7002BAAE672A}"/>
+                    <c16:uniqueId val="{00000001-4D37-42F5-A377-6318DE2B5F0D}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -1034,10 +923,10 @@
                 <c:order val="2"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>[1]Sheet2!$F$3</c15:sqref>
+                          <c15:sqref>Burndown!$H$5</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1059,95 +948,28 @@
                   <a:effectLst/>
                 </c:spPr>
                 <c:marker>
-                  <c:symbol val="triangle"/>
-                  <c:size val="6"/>
-                  <c:spPr>
-                    <a:solidFill>
-                      <a:schemeClr val="accent3"/>
-                    </a:solidFill>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent3"/>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
+                  <c:symbol val="none"/>
                 </c:marker>
-                <c:dLbls>
-                  <c:spPr>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                  <c:txPr>
-                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                      <a:spAutoFit/>
-                    </a:bodyPr>
-                    <a:lstStyle/>
-                    <a:p>
-                      <a:pPr>
-                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="50000"/>
-                              <a:lumOff val="50000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                          <a:latin typeface="+mn-lt"/>
-                          <a:ea typeface="+mn-ea"/>
-                          <a:cs typeface="+mn-cs"/>
-                        </a:defRPr>
-                      </a:pPr>
-                      <a:endParaRPr lang="en-US"/>
-                    </a:p>
-                  </c:txPr>
-                  <c:dLblPos val="t"/>
-                  <c:showLegendKey val="0"/>
-                  <c:showVal val="1"/>
-                  <c:showCatName val="0"/>
-                  <c:showSerName val="0"/>
-                  <c:showPercent val="0"/>
-                  <c:showBubbleSize val="0"/>
-                  <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                      <c15:showLeaderLines val="1"/>
-                      <c15:leaderLines>
-                        <c:spPr>
-                          <a:ln w="9525">
-                            <a:solidFill>
-                              <a:schemeClr val="tx1">
-                                <a:lumMod val="35000"/>
-                                <a:lumOff val="65000"/>
-                              </a:schemeClr>
-                            </a:solidFill>
-                          </a:ln>
-                          <a:effectLst/>
-                        </c:spPr>
-                      </c15:leaderLines>
-                    </c:ext>
-                  </c:extLst>
-                </c:dLbls>
                 <c:cat>
                   <c:multiLvlStrRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>[1]Sheet2!$B$4:$C$5</c15:sqref>
+                          <c15:sqref>Burndown!$D$6:$E$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="2"/>
+                      <c:ptCount val="3"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>    03-01-2021</c:v>
                         </c:pt>
                         <c:pt idx="1">
                           <c:v>    03-17-2021</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>03-29-2021</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -1157,35 +979,41 @@
                         <c:pt idx="1">
                           <c:v>Sprint 1 </c:v>
                         </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Sprint 2</c:v>
+                        </c:pt>
                       </c:lvl>
                     </c:multiLvlStrCache>
                   </c:multiLvlStrRef>
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>[1]Sheet2!$F$4:$F$5</c15:sqref>
+                          <c15:sqref>Burndown!$H$6:$H$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
+                      <c:ptCount val="3"/>
                       <c:pt idx="0">
                         <c:v>0</c:v>
                       </c:pt>
                       <c:pt idx="1">
-                        <c:v>240</c:v>
+                        <c:v>190</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>434</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000002-67FE-497C-B527-7002BAAE672A}"/>
+                    <c16:uniqueId val="{00000002-4D37-42F5-A377-6318DE2B5F0D}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -1196,10 +1024,10 @@
                 <c:order val="3"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>[1]Sheet2!$G$3</c15:sqref>
+                          <c15:sqref>Burndown!$I$5</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1221,93 +1049,28 @@
                   <a:effectLst/>
                 </c:spPr>
                 <c:marker>
-                  <c:symbol val="x"/>
-                  <c:size val="6"/>
-                  <c:spPr>
-                    <a:noFill/>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent4"/>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
+                  <c:symbol val="none"/>
                 </c:marker>
-                <c:dLbls>
-                  <c:spPr>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                  <c:txPr>
-                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                      <a:spAutoFit/>
-                    </a:bodyPr>
-                    <a:lstStyle/>
-                    <a:p>
-                      <a:pPr>
-                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="50000"/>
-                              <a:lumOff val="50000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                          <a:latin typeface="+mn-lt"/>
-                          <a:ea typeface="+mn-ea"/>
-                          <a:cs typeface="+mn-cs"/>
-                        </a:defRPr>
-                      </a:pPr>
-                      <a:endParaRPr lang="en-US"/>
-                    </a:p>
-                  </c:txPr>
-                  <c:dLblPos val="t"/>
-                  <c:showLegendKey val="0"/>
-                  <c:showVal val="1"/>
-                  <c:showCatName val="0"/>
-                  <c:showSerName val="0"/>
-                  <c:showPercent val="0"/>
-                  <c:showBubbleSize val="0"/>
-                  <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                      <c15:showLeaderLines val="1"/>
-                      <c15:leaderLines>
-                        <c:spPr>
-                          <a:ln w="9525">
-                            <a:solidFill>
-                              <a:schemeClr val="tx1">
-                                <a:lumMod val="35000"/>
-                                <a:lumOff val="65000"/>
-                              </a:schemeClr>
-                            </a:solidFill>
-                          </a:ln>
-                          <a:effectLst/>
-                        </c:spPr>
-                      </c15:leaderLines>
-                    </c:ext>
-                  </c:extLst>
-                </c:dLbls>
                 <c:cat>
                   <c:multiLvlStrRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>[1]Sheet2!$B$4:$C$5</c15:sqref>
+                          <c15:sqref>Burndown!$D$6:$E$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="2"/>
+                      <c:ptCount val="3"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>    03-01-2021</c:v>
                         </c:pt>
                         <c:pt idx="1">
                           <c:v>    03-17-2021</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>03-29-2021</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -1317,32 +1080,38 @@
                         <c:pt idx="1">
                           <c:v>Sprint 1 </c:v>
                         </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Sprint 2</c:v>
+                        </c:pt>
                       </c:lvl>
                     </c:multiLvlStrCache>
                   </c:multiLvlStrRef>
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>[1]Sheet2!$G$4:$G$5</c15:sqref>
+                          <c15:sqref>Burndown!$I$6:$I$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
+                      <c:ptCount val="3"/>
                       <c:pt idx="1">
-                        <c:v>480</c:v>
+                        <c:v>300</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>325</c:v>
                       </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000003-67FE-497C-B527-7002BAAE672A}"/>
+                    <c16:uniqueId val="{00000006-4D37-42F5-A377-6318DE2B5F0D}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -1353,10 +1122,10 @@
                 <c:order val="4"/>
                 <c:tx>
                   <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>[1]Sheet2!$H$3</c15:sqref>
+                          <c15:sqref>Burndown!$J$5</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
@@ -1378,93 +1147,28 @@
                   <a:effectLst/>
                 </c:spPr>
                 <c:marker>
-                  <c:symbol val="star"/>
-                  <c:size val="6"/>
-                  <c:spPr>
-                    <a:noFill/>
-                    <a:ln w="9525">
-                      <a:solidFill>
-                        <a:schemeClr val="accent5"/>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
+                  <c:symbol val="none"/>
                 </c:marker>
-                <c:dLbls>
-                  <c:spPr>
-                    <a:noFill/>
-                    <a:ln>
-                      <a:noFill/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                  <c:txPr>
-                    <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                      <a:spAutoFit/>
-                    </a:bodyPr>
-                    <a:lstStyle/>
-                    <a:p>
-                      <a:pPr>
-                        <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="50000"/>
-                              <a:lumOff val="50000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                          <a:latin typeface="+mn-lt"/>
-                          <a:ea typeface="+mn-ea"/>
-                          <a:cs typeface="+mn-cs"/>
-                        </a:defRPr>
-                      </a:pPr>
-                      <a:endParaRPr lang="en-US"/>
-                    </a:p>
-                  </c:txPr>
-                  <c:dLblPos val="t"/>
-                  <c:showLegendKey val="0"/>
-                  <c:showVal val="1"/>
-                  <c:showCatName val="0"/>
-                  <c:showSerName val="0"/>
-                  <c:showPercent val="0"/>
-                  <c:showBubbleSize val="0"/>
-                  <c:showLeaderLines val="0"/>
-                  <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                    <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                      <c15:showLeaderLines val="1"/>
-                      <c15:leaderLines>
-                        <c:spPr>
-                          <a:ln w="9525">
-                            <a:solidFill>
-                              <a:schemeClr val="tx1">
-                                <a:lumMod val="35000"/>
-                                <a:lumOff val="65000"/>
-                              </a:schemeClr>
-                            </a:solidFill>
-                          </a:ln>
-                          <a:effectLst/>
-                        </c:spPr>
-                      </c15:leaderLines>
-                    </c:ext>
-                  </c:extLst>
-                </c:dLbls>
                 <c:cat>
                   <c:multiLvlStrRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>[1]Sheet2!$B$4:$C$5</c15:sqref>
+                          <c15:sqref>Burndown!$D$6:$E$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:multiLvlStrCache>
-                      <c:ptCount val="2"/>
+                      <c:ptCount val="3"/>
                       <c:lvl>
                         <c:pt idx="0">
                           <c:v>    03-01-2021</c:v>
                         </c:pt>
                         <c:pt idx="1">
                           <c:v>    03-17-2021</c:v>
+                        </c:pt>
+                        <c:pt idx="2">
+                          <c:v>03-29-2021</c:v>
                         </c:pt>
                       </c:lvl>
                       <c:lvl>
@@ -1474,29 +1178,38 @@
                         <c:pt idx="1">
                           <c:v>Sprint 1 </c:v>
                         </c:pt>
+                        <c:pt idx="2">
+                          <c:v>Sprint 2</c:v>
+                        </c:pt>
                       </c:lvl>
                     </c:multiLvlStrCache>
                   </c:multiLvlStrRef>
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                    <c:extLst>
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
-                          <c15:sqref>[1]Sheet2!$H$4:$H$5</c15:sqref>
+                          <c15:sqref>Burndown!$J$6:$J$8</c15:sqref>
                         </c15:formulaRef>
                       </c:ext>
                     </c:extLst>
                     <c:numCache>
                       <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="2"/>
+                      <c:ptCount val="3"/>
+                      <c:pt idx="1">
+                        <c:v>38</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>80.069999999999993</c:v>
+                      </c:pt>
                     </c:numCache>
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                <c:extLst>
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000004-67FE-497C-B527-7002BAAE672A}"/>
+                    <c16:uniqueId val="{00000007-4D37-42F5-A377-6318DE2B5F0D}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -1505,10 +1218,11 @@
         </c:extLst>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="145513856"/>
+        <c:axId val="516104256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
@@ -1545,12 +1259,20 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-IN"/>
-                  <a:t>dates</a:t>
+                  <a:t>Dates</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.44583202099737529"/>
+              <c:y val="0.89719889180519097"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1558,9 +1280,30 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1595,17 +1338,19 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145552896"/>
+        <c:crossAx val="516110488"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145552896"/>
+        <c:axId val="516110488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
+        <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:title>
           <c:tx>
@@ -1627,10 +1372,9 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-IN" baseline="0"/>
-                  <a:t>rEMAINING stories</a:t>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Remaining Stories</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-IN"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -1638,10 +1382,11 @@
             <c:manualLayout>
               <c:xMode val="edge"/>
               <c:yMode val="edge"/>
-              <c:x val="1.6666666666666673E-2"/>
-              <c:y val="0.30253827646544196"/>
+              <c:x val="1.6666666666666666E-2"/>
+              <c:y val="0.27049394867308257"/>
             </c:manualLayout>
           </c:layout>
+          <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
             <a:ln>
@@ -1649,9 +1394,30 @@
             </a:ln>
             <a:effectLst/>
           </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
@@ -1686,7 +1452,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="145513856"/>
+        <c:crossAx val="516104256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1698,46 +1464,16 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:layout/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="zero"/>
-    <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+    <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
           <c16r3:dispNaAsBlank val="1"/>
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
+    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -1766,7 +1502,7 @@
   </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2338,28 +2074,26 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>396875</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>92075</xdr:rowOff>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>73025</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>365125</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DD35CEC-24C0-4E18-8138-631ACCAB9487}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CA6A969-60A6-4116-B9E2-26C869B4D1B6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr>
-          <a:graphicFrameLocks/>
-        </xdr:cNvGraphicFramePr>
+        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -2377,7 +2111,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Sheet1"/>
@@ -2488,7 +2222,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2520,9 +2254,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2554,6 +2306,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2729,123 +2499,123 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:F11"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="29.28515625" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" customWidth="1"/>
+    <col min="3" max="4" width="11.26953125" customWidth="1"/>
+    <col min="5" max="5" width="29.26953125" customWidth="1"/>
+    <col min="6" max="6" width="27.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="18.75">
+    <row r="3" spans="2:6" ht="18.5" x14ac:dyDescent="0.45">
       <c r="E3" s="21" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1"/>
-    <row r="5" spans="2:6">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B5" s="12" t="s">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>47</v>
+        <v>30</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B8" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6">
-      <c r="B7" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6">
-      <c r="B8" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>35</v>
-      </c>
       <c r="D8" s="7" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>33</v>
+        <v>16</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B9" s="8" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B10" s="8"/>
       <c r="C10" s="7"/>
       <c r="D10" s="7"/>
       <c r="E10" s="6" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" ht="15.75" thickBot="1">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="4"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
@@ -2854,10 +2624,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E9" r:id="rId1"/>
-    <hyperlink ref="E8" r:id="rId2"/>
-    <hyperlink ref="E7" r:id="rId3"/>
-    <hyperlink ref="E6" r:id="rId4"/>
+    <hyperlink ref="E9" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E8" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E7" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
@@ -2865,327 +2635,462 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="30.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.81640625" customWidth="1"/>
+    <col min="6" max="6" width="30.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="17"/>
-      <c r="F2" s="24" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="F2" s="21" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="17"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="17"/>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="17"/>
       <c r="C5" s="17">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A6" s="17"/>
-      <c r="C6" s="17">
-        <v>1</v>
-      </c>
+      <c r="C6" s="17"/>
       <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>102</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="17"/>
       <c r="C7" s="17">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>15</v>
-      </c>
       <c r="F7" t="s">
-        <v>14</v>
+        <v>61</v>
       </c>
       <c r="G7" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="17"/>
-      <c r="C8" s="17">
-        <v>1</v>
-      </c>
+      <c r="C8" s="17"/>
       <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>103</v>
+      </c>
+      <c r="F8" s="22" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="17"/>
       <c r="C9" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="G9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="C10" s="17">
-        <v>1</v>
-      </c>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="72.5" x14ac:dyDescent="0.35">
+      <c r="A10" s="17"/>
+      <c r="C10" s="17"/>
       <c r="D10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" t="s">
-        <v>7</v>
-      </c>
-      <c r="F10" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>104</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A11" s="17"/>
       <c r="C11" s="17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>5</v>
+        <v>55</v>
       </c>
       <c r="E11" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="F11" t="s">
-        <v>4</v>
+        <v>63</v>
       </c>
       <c r="G11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="C12" s="17">
-        <v>1</v>
-      </c>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A12" s="17"/>
+      <c r="C12" s="17"/>
       <c r="D12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" t="s">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="C13" s="17">
-        <v>2</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A13" s="17"/>
+      <c r="C13" s="17"/>
       <c r="D13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E13" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" t="s">
-        <v>85</v>
-      </c>
-      <c r="G13" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="C14" s="17">
-        <v>2</v>
-      </c>
+        <v>107</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A14" s="17"/>
+      <c r="C14" s="17"/>
       <c r="D14" t="s">
-        <v>78</v>
-      </c>
-      <c r="E14" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" t="s">
-        <v>86</v>
-      </c>
-      <c r="G14" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>108</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15" s="17"/>
       <c r="C15" s="17">
         <v>2</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="E15" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>87</v>
+        <v>109</v>
       </c>
       <c r="G15" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="C16" s="17">
-        <v>2</v>
-      </c>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="17"/>
+      <c r="C16" s="17"/>
       <c r="D16" t="s">
-        <v>80</v>
-      </c>
-      <c r="E16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" t="s">
-        <v>88</v>
-      </c>
-      <c r="G16" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:7">
-      <c r="C17" s="17">
-        <v>2</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="17"/>
+      <c r="C17" s="17"/>
       <c r="D17" t="s">
-        <v>81</v>
-      </c>
-      <c r="E17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" t="s">
-        <v>89</v>
-      </c>
-      <c r="G17" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="3:7">
-      <c r="C18" s="17">
-        <v>2</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="17"/>
+      <c r="C18" s="17"/>
       <c r="D18" t="s">
-        <v>82</v>
-      </c>
-      <c r="E18" t="s">
-        <v>15</v>
-      </c>
-      <c r="F18" t="s">
-        <v>90</v>
-      </c>
-      <c r="G18" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="3:7">
+        <v>114</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="C19" s="17">
         <v>2</v>
       </c>
       <c r="D19" t="s">
-        <v>83</v>
+        <v>57</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F19" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="C20" s="17"/>
+      <c r="D20" t="s">
+        <v>115</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="C21" s="17"/>
+      <c r="D21" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C22" s="17">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>58</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>66</v>
+      </c>
+      <c r="G22" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="C23" s="17"/>
+      <c r="D23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C24" s="17">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>67</v>
+      </c>
+      <c r="G24" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C25" s="17"/>
+      <c r="D25" t="s">
+        <v>120</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="C26" s="17"/>
+      <c r="D26" t="s">
+        <v>122</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C27" s="17">
+        <v>3</v>
+      </c>
+      <c r="D27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" t="s">
+        <v>90</v>
+      </c>
+      <c r="G27" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C28" s="17">
+        <v>3</v>
+      </c>
+      <c r="D28" t="s">
+        <v>53</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
         <v>91</v>
       </c>
-      <c r="G19" t="s">
+      <c r="G28" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="3:7">
-      <c r="C20" s="17">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C29" s="17">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
+        <v>54</v>
+      </c>
+      <c r="E29" t="s">
+        <v>4</v>
+      </c>
+      <c r="F29" t="s">
+        <v>92</v>
+      </c>
+      <c r="G29" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C30" s="17">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
+        <v>55</v>
+      </c>
+      <c r="E30" t="s">
+        <v>4</v>
+      </c>
+      <c r="F30" t="s">
+        <v>93</v>
+      </c>
+      <c r="G30" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C31" s="17">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" t="s">
+        <v>3</v>
+      </c>
+      <c r="F31" t="s">
+        <v>94</v>
+      </c>
+      <c r="G31" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C32" s="17">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
+        <v>57</v>
+      </c>
+      <c r="E32" t="s">
+        <v>3</v>
+      </c>
+      <c r="F32" t="s">
+        <v>95</v>
+      </c>
+      <c r="G32" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C33" s="17">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>58</v>
+      </c>
+      <c r="E33" t="s">
         <v>2</v>
       </c>
-      <c r="D20" t="s">
-        <v>84</v>
-      </c>
-      <c r="E20" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" t="s">
-        <v>92</v>
-      </c>
-      <c r="G20" t="s">
+      <c r="F33" t="s">
+        <v>96</v>
+      </c>
+      <c r="G33" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C34" s="17">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
+        <v>59</v>
+      </c>
+      <c r="E34" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>97</v>
+      </c>
+      <c r="G34" t="s">
         <v>0</v>
       </c>
     </row>
@@ -3196,59 +3101,59 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="D2:K7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="D2:K8"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
-    <col min="5" max="5" width="14.28515625" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.28515625" customWidth="1"/>
+    <col min="4" max="4" width="10.26953125" customWidth="1"/>
+    <col min="5" max="5" width="14.26953125" customWidth="1"/>
+    <col min="6" max="6" width="19.26953125" customWidth="1"/>
+    <col min="7" max="7" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" customWidth="1"/>
+    <col min="10" max="10" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:11" ht="18.75">
+    <row r="2" spans="4:11" ht="18.5" x14ac:dyDescent="0.45">
       <c r="F2" s="20" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="5" spans="4:11">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="5" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D5" s="15" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="E5" s="15" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="4:11">
+    <row r="6" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D6" t="s">
-        <v>55</v>
+        <v>38</v>
       </c>
       <c r="E6" s="18" t="s">
-        <v>56</v>
+        <v>39</v>
       </c>
       <c r="F6" s="17">
         <v>32</v>
@@ -3257,12 +3162,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="4:11">
+    <row r="7" spans="4:11" x14ac:dyDescent="0.35">
       <c r="D7" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="E7" s="14" t="s">
-        <v>58</v>
+        <v>41</v>
       </c>
       <c r="F7" s="17">
         <v>24</v>
@@ -3278,6 +3183,29 @@
       </c>
       <c r="J7" s="17">
         <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="4:11" x14ac:dyDescent="0.35">
+      <c r="D8" t="s">
+        <v>77</v>
+      </c>
+      <c r="E8" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="17">
+        <v>16</v>
+      </c>
+      <c r="G8" s="17">
+        <v>8</v>
+      </c>
+      <c r="H8" s="17">
+        <v>434</v>
+      </c>
+      <c r="I8" s="17">
+        <v>325</v>
+      </c>
+      <c r="J8" s="17">
+        <v>80.069999999999993</v>
       </c>
     </row>
   </sheetData>
@@ -3287,655 +3215,317 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="E2:M45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="E2:M22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="10.28515625" customWidth="1"/>
-    <col min="6" max="6" width="43.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="3" max="3" width="10.26953125" customWidth="1"/>
+    <col min="6" max="6" width="43.1796875" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" customWidth="1"/>
+    <col min="13" max="13" width="14.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="5:13" ht="18.75">
+    <row r="2" spans="5:13" ht="18.5" x14ac:dyDescent="0.45">
       <c r="F2" s="21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="5:13">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="5" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E5" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>59</v>
+        <v>42</v>
       </c>
       <c r="J5" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" t="s">
         <v>60</v>
       </c>
-      <c r="K5" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M5" s="1" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="6" spans="5:13">
-      <c r="E6" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" t="s">
-        <v>64</v>
-      </c>
       <c r="G6" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="I6" s="17">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="J6" s="17">
         <v>60</v>
       </c>
       <c r="K6" s="17">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="L6" s="17">
-        <v>25</v>
+        <v>60</v>
       </c>
       <c r="M6" s="19" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="7" spans="5:13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E7" t="s">
-        <v>140</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>141</v>
+        <v>61</v>
       </c>
       <c r="G7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="17"/>
-      <c r="M7" s="19"/>
-    </row>
-    <row r="8" spans="5:13">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="17">
+        <v>30</v>
+      </c>
+      <c r="J7" s="17">
+        <v>60</v>
+      </c>
+      <c r="K7" s="17">
+        <v>22</v>
+      </c>
+      <c r="L7" s="17">
+        <v>60</v>
+      </c>
+      <c r="M7" s="19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E8" t="s">
-        <v>138</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>142</v>
+        <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17"/>
-      <c r="M8" s="19"/>
-    </row>
-    <row r="9" spans="5:13" ht="30">
+        <v>4</v>
+      </c>
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="I8" s="17">
+        <v>70</v>
+      </c>
+      <c r="J8" s="17">
+        <v>80</v>
+      </c>
+      <c r="K8" s="17">
+        <v>85</v>
+      </c>
+      <c r="L8" s="17">
+        <v>78</v>
+      </c>
+      <c r="M8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E9" t="s">
-        <v>134</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>143</v>
+        <v>55</v>
+      </c>
+      <c r="F9" t="s">
+        <v>63</v>
       </c>
       <c r="G9" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="19"/>
-    </row>
-    <row r="10" spans="5:13">
+        <v>4</v>
+      </c>
+      <c r="H9" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="17">
+        <v>130</v>
+      </c>
+      <c r="J9" s="17">
+        <v>128</v>
+      </c>
+      <c r="K9" s="17">
+        <v>60</v>
+      </c>
+      <c r="L9" s="17">
+        <v>63</v>
+      </c>
+      <c r="M9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E10" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G10" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="H10" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="I10" s="17">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="J10" s="17">
         <v>60</v>
       </c>
       <c r="K10" s="17">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="L10" s="17">
-        <v>30</v>
-      </c>
-      <c r="M10" s="19" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="5:13">
+        <v>34</v>
+      </c>
+      <c r="M10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E11" t="s">
-        <v>136</v>
+        <v>57</v>
       </c>
       <c r="F11" t="s">
-        <v>137</v>
+        <v>65</v>
       </c>
       <c r="G11" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="M11" s="19"/>
-    </row>
-    <row r="12" spans="5:13">
+        <v>3</v>
+      </c>
+      <c r="H11" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="17">
+        <v>60</v>
+      </c>
+      <c r="J11" s="17">
+        <v>20</v>
+      </c>
+      <c r="K11" s="17">
+        <v>68</v>
+      </c>
+      <c r="L11" s="17">
+        <v>10</v>
+      </c>
+      <c r="M11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E12" t="s">
-        <v>138</v>
+        <v>81</v>
       </c>
       <c r="F12" t="s">
-        <v>139</v>
+        <v>66</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="M12" s="19"/>
-    </row>
-    <row r="13" spans="5:13">
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="17">
+        <v>10</v>
+      </c>
+      <c r="J12" s="17">
+        <v>10</v>
+      </c>
+      <c r="K12" s="17">
+        <v>5</v>
+      </c>
+      <c r="L12" s="17">
+        <v>5</v>
+      </c>
+      <c r="M12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="5:13" x14ac:dyDescent="0.35">
       <c r="E13" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="F13" t="s">
         <v>67</v>
       </c>
       <c r="G13" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="H13" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="I13" s="17">
         <v>30</v>
       </c>
       <c r="J13" s="17">
-        <v>60</v>
+        <v>30</v>
       </c>
       <c r="K13" s="17">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="L13" s="17">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="M13" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="14" spans="5:13">
-      <c r="E14" t="s">
-        <v>130</v>
-      </c>
-      <c r="F14" t="s">
-        <v>131</v>
-      </c>
-      <c r="G14" t="s">
-        <v>15</v>
-      </c>
-      <c r="I14" s="17"/>
-      <c r="J14" s="17"/>
-      <c r="K14" s="17"/>
-      <c r="L14" s="17"/>
-    </row>
-    <row r="15" spans="5:13">
-      <c r="E15" t="s">
-        <v>132</v>
-      </c>
-      <c r="F15" t="s">
-        <v>133</v>
-      </c>
-      <c r="G15" t="s">
-        <v>15</v>
-      </c>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="17"/>
-    </row>
-    <row r="16" spans="5:13">
-      <c r="E16" t="s">
-        <v>134</v>
-      </c>
-      <c r="F16" t="s">
-        <v>135</v>
-      </c>
-      <c r="G16" t="s">
-        <v>15</v>
-      </c>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-    </row>
-    <row r="17" spans="5:13">
-      <c r="E17" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G17" t="s">
-        <v>15</v>
-      </c>
-      <c r="H17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="5:13" x14ac:dyDescent="0.35">
+      <c r="E16" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="I17" s="17">
-        <v>30</v>
-      </c>
-      <c r="J17" s="17">
-        <v>60</v>
-      </c>
-      <c r="K17" s="17">
-        <v>22</v>
-      </c>
-      <c r="L17" s="17">
-        <v>30</v>
-      </c>
-      <c r="M17" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="5:13">
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E17" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E18" t="s">
-        <v>123</v>
-      </c>
-      <c r="F18" t="s">
-        <v>125</v>
-      </c>
-      <c r="G18" t="s">
-        <v>15</v>
-      </c>
-      <c r="I18" s="17"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="17"/>
-      <c r="L18" s="17"/>
-    </row>
-    <row r="19" spans="5:13" ht="30">
-      <c r="E19" t="s">
-        <v>126</v>
-      </c>
-      <c r="F19" s="22" t="s">
-        <v>129</v>
-      </c>
-      <c r="G19" t="s">
-        <v>15</v>
-      </c>
-      <c r="I19" s="17"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="17"/>
-      <c r="L19" s="17"/>
-    </row>
-    <row r="20" spans="5:13">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E20" t="s">
-        <v>127</v>
-      </c>
-      <c r="F20" t="s">
-        <v>128</v>
-      </c>
-      <c r="G20" t="s">
-        <v>15</v>
-      </c>
-      <c r="I20" s="17"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="17"/>
-      <c r="L20" s="17"/>
-    </row>
-    <row r="21" spans="5:13">
-      <c r="E21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" t="s">
-        <v>9</v>
-      </c>
-      <c r="G21" t="s">
-        <v>7</v>
-      </c>
-      <c r="H21" t="s">
-        <v>72</v>
-      </c>
-      <c r="I21" s="17">
-        <v>30</v>
-      </c>
-      <c r="J21" s="17">
-        <v>60</v>
-      </c>
-      <c r="K21" s="17">
-        <v>18</v>
-      </c>
-      <c r="L21" s="17">
-        <v>45</v>
-      </c>
-      <c r="M21" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="22" spans="5:13">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="5:6" x14ac:dyDescent="0.35">
+      <c r="E21" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E22" t="s">
-        <v>116</v>
-      </c>
-      <c r="F22" t="s">
-        <v>144</v>
-      </c>
-      <c r="G22" t="s">
-        <v>7</v>
-      </c>
-      <c r="I22" s="17"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="17"/>
-      <c r="L22" s="17"/>
-    </row>
-    <row r="23" spans="5:13">
-      <c r="E23" t="s">
-        <v>122</v>
-      </c>
-      <c r="F23" t="s">
-        <v>145</v>
-      </c>
-      <c r="G23" t="s">
-        <v>7</v>
-      </c>
-      <c r="I23" s="17"/>
-      <c r="J23" s="17"/>
-      <c r="K23" s="17"/>
-      <c r="L23" s="17"/>
-    </row>
-    <row r="24" spans="5:13">
-      <c r="E24" t="s">
-        <v>146</v>
-      </c>
-      <c r="F24" t="s">
-        <v>147</v>
-      </c>
-      <c r="G24" t="s">
-        <v>7</v>
-      </c>
-      <c r="I24" s="17"/>
-      <c r="J24" s="17"/>
-      <c r="K24" s="17"/>
-      <c r="L24" s="17"/>
-    </row>
-    <row r="25" spans="5:13">
-      <c r="E25" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" t="s">
-        <v>6</v>
-      </c>
-      <c r="G25" t="s">
-        <v>7</v>
-      </c>
-      <c r="H25" t="s">
-        <v>72</v>
-      </c>
-      <c r="I25" s="17">
-        <v>30</v>
-      </c>
-      <c r="J25" s="17">
-        <v>60</v>
-      </c>
-      <c r="K25" s="17">
-        <v>20</v>
-      </c>
-      <c r="L25" s="17">
-        <v>60</v>
-      </c>
-      <c r="M25" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="26" spans="5:13">
-      <c r="E26" t="s">
-        <v>110</v>
-      </c>
-      <c r="F26" t="s">
-        <v>111</v>
-      </c>
-      <c r="G26" t="s">
-        <v>7</v>
-      </c>
-      <c r="I26" s="17"/>
-      <c r="J26" s="17"/>
-      <c r="K26" s="17"/>
-      <c r="L26" s="17"/>
-    </row>
-    <row r="27" spans="5:13">
-      <c r="E27" t="s">
-        <v>112</v>
-      </c>
-      <c r="F27" t="s">
-        <v>113</v>
-      </c>
-      <c r="G27" t="s">
-        <v>7</v>
-      </c>
-      <c r="I27" s="17"/>
-      <c r="J27" s="17"/>
-      <c r="K27" s="17"/>
-      <c r="L27" s="17"/>
-    </row>
-    <row r="28" spans="5:13">
-      <c r="E28" t="s">
-        <v>114</v>
-      </c>
-      <c r="F28" t="s">
-        <v>115</v>
-      </c>
-      <c r="G28" t="s">
-        <v>7</v>
-      </c>
-      <c r="I28" s="17"/>
-      <c r="J28" s="17"/>
-      <c r="K28" s="17"/>
-      <c r="L28" s="17"/>
-    </row>
-    <row r="29" spans="5:13">
-      <c r="E29" t="s">
-        <v>68</v>
-      </c>
-      <c r="F29" t="s">
-        <v>69</v>
-      </c>
-      <c r="G29" t="s">
-        <v>2</v>
-      </c>
-      <c r="H29" t="s">
-        <v>72</v>
-      </c>
-      <c r="I29" s="17">
-        <v>30</v>
-      </c>
-      <c r="J29" s="17">
-        <v>60</v>
-      </c>
-      <c r="K29" s="17">
-        <v>35</v>
-      </c>
-      <c r="L29" s="17">
-        <v>30</v>
-      </c>
-      <c r="M29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="5:13" ht="30">
-      <c r="E30" t="s">
-        <v>104</v>
-      </c>
-      <c r="F30" s="22" t="s">
-        <v>105</v>
-      </c>
-      <c r="G30" t="s">
-        <v>2</v>
-      </c>
-      <c r="I30" s="17"/>
-      <c r="J30" s="17"/>
-      <c r="K30" s="17"/>
-      <c r="L30" s="17"/>
-    </row>
-    <row r="31" spans="5:13">
-      <c r="E31" t="s">
-        <v>106</v>
-      </c>
-      <c r="F31" t="s">
-        <v>107</v>
-      </c>
-      <c r="G31" t="s">
-        <v>2</v>
-      </c>
-      <c r="I31" s="17"/>
-      <c r="J31" s="17"/>
-      <c r="K31" s="17"/>
-      <c r="L31" s="17"/>
-    </row>
-    <row r="32" spans="5:13" ht="30">
-      <c r="E32" t="s">
-        <v>108</v>
-      </c>
-      <c r="F32" s="22" t="s">
-        <v>109</v>
-      </c>
-      <c r="G32" t="s">
-        <v>2</v>
-      </c>
-      <c r="I32" s="17"/>
-      <c r="J32" s="17"/>
-      <c r="K32" s="17"/>
-      <c r="L32" s="17"/>
-    </row>
-    <row r="33" spans="5:13">
-      <c r="E33" t="s">
-        <v>3</v>
-      </c>
-      <c r="F33" t="s">
-        <v>70</v>
-      </c>
-      <c r="G33" t="s">
-        <v>2</v>
-      </c>
-      <c r="H33" t="s">
-        <v>72</v>
-      </c>
-      <c r="I33" s="17">
-        <v>30</v>
-      </c>
-      <c r="J33" s="17">
-        <v>60</v>
-      </c>
-      <c r="K33" s="17">
-        <v>25</v>
-      </c>
-      <c r="L33" s="17">
-        <v>60</v>
-      </c>
-      <c r="M33" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="5:13">
-      <c r="E34" t="s">
-        <v>98</v>
-      </c>
-      <c r="F34" t="s">
-        <v>99</v>
-      </c>
-      <c r="G34" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="35" spans="5:13">
-      <c r="E35" t="s">
-        <v>100</v>
-      </c>
-      <c r="F35" t="s">
-        <v>101</v>
-      </c>
-      <c r="G35" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="36" spans="5:13" ht="30">
-      <c r="E36" t="s">
-        <v>102</v>
-      </c>
-      <c r="F36" s="22" t="s">
-        <v>103</v>
-      </c>
-      <c r="G36" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="39" spans="5:13">
-      <c r="E39" s="1" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="40" spans="5:13">
-      <c r="E40" s="1" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="41" spans="5:13">
-      <c r="E41" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="43" spans="5:13">
-      <c r="E43" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="44" spans="5:13">
-      <c r="E44" s="1" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="45" spans="5:13">
-      <c r="E45" t="s">
-        <v>121</v>
-      </c>
-      <c r="F45" s="23"/>
+        <v>75</v>
+      </c>
+      <c r="F22" s="23"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3944,174 +3534,174 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="D2:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="5" max="5" width="10.140625" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" customWidth="1"/>
-    <col min="7" max="7" width="52.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.1796875" customWidth="1"/>
+    <col min="6" max="6" width="10.26953125" customWidth="1"/>
+    <col min="7" max="7" width="52.453125" customWidth="1"/>
+    <col min="8" max="8" width="11.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:8" ht="18.75">
+    <row r="2" spans="4:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="G2" s="21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="4:8">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D4" s="1" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="4:8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D5" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="F5" t="s">
         <v>2</v>
       </c>
       <c r="G5" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="H5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="4:8">
+    <row r="6" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D6" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E6" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="F6" t="s">
         <v>2</v>
       </c>
       <c r="G6" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="H6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="4:8">
+    <row r="7" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D7" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="H7" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="4:8">
+    <row r="8" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D8" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E8" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G8" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="H8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="4:8">
+    <row r="9" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D9" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E9" t="s">
-        <v>81</v>
+        <v>86</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G9" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="H9" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="4:8">
+    <row r="10" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D10" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E10" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="H10" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="4:8">
+    <row r="11" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D11" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="F11" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G11" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="H11" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="4:8">
+    <row r="12" spans="4:8" x14ac:dyDescent="0.35">
       <c r="D12" s="17">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="F12" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G12" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="H12" t="s">
         <v>0</v>

</xml_diff>